<commit_message>
Prepared September schedule, qPCR group and run lists. Continued work on Flying or Not Flying data analysis scripts.
</commit_message>
<xml_diff>
--- a/data/raw/Flying/Samples-Flying.xlsx
+++ b/data/raw/Flying/Samples-Flying.xlsx
@@ -35,6 +35,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Had pollen</t>
         </r>
@@ -62,7 +63,7 @@
     <t xml:space="preserve">Flying</t>
   </si>
   <si>
-    <t xml:space="preserve">001</t>
+    <t xml:space="preserve">Fly_001</t>
   </si>
   <si>
     <t xml:space="preserve">Ca</t>
@@ -77,127 +78,127 @@
     <t xml:space="preserve">F</t>
   </si>
   <si>
-    <t xml:space="preserve">002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">003</t>
+    <t xml:space="preserve">Fly_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_003</t>
   </si>
   <si>
     <t xml:space="preserve">T</t>
   </si>
   <si>
-    <t xml:space="preserve">004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">021</t>
+    <t xml:space="preserve">Fly_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_021</t>
   </si>
   <si>
     <t xml:space="preserve">Ib</t>
   </si>
   <si>
-    <t xml:space="preserve">022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">035</t>
-  </si>
-  <si>
-    <t xml:space="preserve">036</t>
-  </si>
-  <si>
-    <t xml:space="preserve">037</t>
-  </si>
-  <si>
-    <t xml:space="preserve">038</t>
-  </si>
-  <si>
-    <t xml:space="preserve">039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">040</t>
+    <t xml:space="preserve">Fly_022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_036</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_037</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fly_040</t>
   </si>
 </sst>
 </file>
@@ -213,6 +214,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -317,10 +319,10 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -343,16 +345,16 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -360,16 +362,16 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -377,16 +379,16 @@
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -394,16 +396,16 @@
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -411,16 +413,16 @@
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -428,16 +430,16 @@
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -445,16 +447,16 @@
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="0" t="s">
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -462,16 +464,16 @@
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -479,16 +481,16 @@
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="0" t="s">
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -496,16 +498,16 @@
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -513,16 +515,16 @@
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -530,16 +532,16 @@
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -547,16 +549,16 @@
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -564,16 +566,16 @@
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="0" t="s">
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -581,16 +583,16 @@
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -598,16 +600,16 @@
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="0" t="s">
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -615,16 +617,16 @@
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="0" t="s">
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -632,16 +634,16 @@
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="0" t="s">
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -649,16 +651,16 @@
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="0" t="s">
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -666,16 +668,16 @@
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="0" t="s">
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -683,16 +685,16 @@
       <c r="A22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="0" t="n">
+      <c r="B22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="0" t="s">
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -700,16 +702,16 @@
       <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="0" t="n">
+      <c r="B23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="0" t="s">
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -717,16 +719,16 @@
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="0" t="n">
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="0" t="s">
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -734,16 +736,16 @@
       <c r="A25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="0" t="n">
+      <c r="B25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="0" t="s">
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -751,16 +753,16 @@
       <c r="A26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="0" t="n">
+      <c r="B26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="0" t="s">
+      <c r="D26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -768,16 +770,16 @@
       <c r="A27" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="0" t="n">
+      <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="0" t="s">
+      <c r="D27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -785,16 +787,16 @@
       <c r="A28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="0" t="n">
+      <c r="B28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="0" t="s">
+      <c r="D28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -802,16 +804,16 @@
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="0" t="n">
+      <c r="B29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="0" t="s">
+      <c r="D29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -819,16 +821,16 @@
       <c r="A30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="0" t="n">
+      <c r="B30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="0" t="s">
+      <c r="D30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -836,16 +838,16 @@
       <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="0" t="n">
+      <c r="B31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="0" t="s">
+      <c r="D31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -853,16 +855,16 @@
       <c r="A32" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="0" t="n">
+      <c r="B32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="0" t="s">
+      <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -870,16 +872,16 @@
       <c r="A33" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="0" t="n">
+      <c r="B33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="0" t="s">
+      <c r="D33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -887,16 +889,16 @@
       <c r="A34" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="0" t="n">
+      <c r="B34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="0" t="s">
+      <c r="D34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -904,16 +906,16 @@
       <c r="A35" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B35" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="0" t="n">
+      <c r="B35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="0" t="s">
+      <c r="D35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -921,16 +923,16 @@
       <c r="A36" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="0" t="n">
+      <c r="B36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="D36" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="0" t="s">
+      <c r="D36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -938,16 +940,16 @@
       <c r="A37" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C37" s="0" t="n">
+      <c r="B37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="0" t="s">
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -955,16 +957,16 @@
       <c r="A38" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="0" t="n">
+      <c r="B38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="D38" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="0" t="s">
+      <c r="D38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -972,16 +974,16 @@
       <c r="A39" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="0" t="n">
+      <c r="B39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="D39" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="0" t="s">
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -989,16 +991,16 @@
       <c r="A40" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="0" t="n">
+      <c r="B40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="D40" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="0" t="s">
+      <c r="D40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1006,16 +1008,16 @@
       <c r="A41" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="0" t="n">
+      <c r="B41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="D41" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="0" t="s">
+      <c r="D41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>